<commit_message>
Now aligned to syntax X,Y,Z for calibration and simulation procedure explanation
</commit_message>
<xml_diff>
--- a/data/Single_row.xlsx
+++ b/data/Single_row.xlsx
@@ -230,7 +230,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -254,15 +254,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
       <b/>
     </font>
   </fonts>
@@ -295,7 +286,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>

<commit_message>
Included ACF cumulative losses bvreak down and improved calibration.
</commit_message>
<xml_diff>
--- a/data/Single_row.xlsx
+++ b/data/Single_row.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JFV09\Dropbox\Git\india-subnational\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1D34BF-9620-4BEB-AC14-38E3BC6CCB40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12735" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="X" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Y" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Z" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="I" sheetId="5" state="visible" r:id="rId4"/>
+    <sheet name="X" sheetId="1" r:id="rId1"/>
+    <sheet name="Y" sheetId="2" r:id="rId2"/>
+    <sheet name="Z" sheetId="3" r:id="rId3"/>
+    <sheet name="I" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
   <si>
     <t>beta</t>
   </si>
@@ -223,14 +230,19 @@
   </si>
   <si>
     <t>0.5 # Operational losses on expected yield</t>
+  </si>
+  <si>
+    <t>pop2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -239,22 +251,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <b/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <b/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -274,24 +301,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -599,16 +631,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -639,37 +671,43 @@
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="K1" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>415.12270000000001</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>384.78899999999999</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>84</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>0.1</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>6.0439999999999994E-2</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>0.1</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>0.1</v>
+      </c>
+      <c r="K2">
+        <v>4625525.533747999</v>
       </c>
     </row>
   </sheetData>
@@ -679,143 +717,143 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="n">
-        <v>4.5002542958438401</v>
-      </c>
-      <c r="D2" t="n">
-        <v>3.9906912958829199</v>
-      </c>
-      <c r="E2" t="n">
-        <v>14.1541794979284</v>
-      </c>
-      <c r="F2" t="n">
-        <v>9.5318065851973596E-2</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.86014316604833996</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.79401565427736598</v>
-      </c>
-      <c r="I2" t="n">
-        <v>11.265009956511401</v>
-      </c>
-      <c r="J2" t="n">
-        <v>4.9314238565595501</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.258660516444849</v>
-      </c>
-      <c r="L2" t="n">
-        <v>2.01651831734533</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.43549678661083902</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.21222864011010001</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.219496571163387</v>
-      </c>
-      <c r="P2" t="n">
-        <v>5.1738444306207103E-2</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.39212459986411202</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0.95696942592508005</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.74436917548180503</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1.56396914678005E-3</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.25314412502269401</v>
+      <c r="C2">
+        <v>6.5270526608800097</v>
+      </c>
+      <c r="D2">
+        <v>7.8938477584069204</v>
+      </c>
+      <c r="E2">
+        <v>5.8020587178346901</v>
+      </c>
+      <c r="F2">
+        <v>0.15019495458955001</v>
+      </c>
+      <c r="G2">
+        <v>2.3709421724155502</v>
+      </c>
+      <c r="H2">
+        <v>3.3789478987042498</v>
+      </c>
+      <c r="I2">
+        <v>8.7993595924772503</v>
+      </c>
+      <c r="J2">
+        <v>4.1256173617156602</v>
+      </c>
+      <c r="K2">
+        <v>0.59606479204033702</v>
+      </c>
+      <c r="L2">
+        <v>5.9956278734424799</v>
+      </c>
+      <c r="M2">
+        <v>0.39044616397628901</v>
+      </c>
+      <c r="N2">
+        <v>0.16326516547973699</v>
+      </c>
+      <c r="O2">
+        <v>0.15874636396962799</v>
+      </c>
+      <c r="P2">
+        <v>0.26087663656740101</v>
+      </c>
+      <c r="Q2">
+        <v>0.31970460359210101</v>
+      </c>
+      <c r="R2">
+        <v>0.89453394849780199</v>
+      </c>
+      <c r="S2">
+        <v>0.770749447658161</v>
+      </c>
+      <c r="T2">
+        <v>0.58009231533213201</v>
+      </c>
+      <c r="U2">
+        <v>0.30786970724652202</v>
       </c>
     </row>
   </sheetData>
@@ -825,256 +863,262 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="19" max="20" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="n">
-        <v>384.741596529298</v>
-      </c>
-      <c r="D2" t="n">
-        <v>333.738952016604</v>
-      </c>
-      <c r="E2" t="n">
-        <v>186.687123745202</v>
-      </c>
-      <c r="F2" t="n">
-        <v>110.549943914274</v>
-      </c>
-      <c r="G2" t="n">
-        <v>82.5940956676615</v>
-      </c>
-      <c r="H2" t="n">
-        <v>71.1285070176593</v>
-      </c>
-      <c r="I2" t="n">
-        <v>63.7072135540608</v>
-      </c>
-      <c r="J2" t="n">
-        <v>58.7387558793581</v>
-      </c>
-      <c r="K2" t="n">
-        <v>83.459540056375</v>
-      </c>
-      <c r="L2" t="n">
-        <v>80.8371545830991</v>
-      </c>
-      <c r="M2" t="n">
-        <v>62.3777091835037</v>
-      </c>
-      <c r="N2" t="n">
-        <v>40.292855193487</v>
-      </c>
-      <c r="O2" t="n">
-        <v>26.7164941704349</v>
-      </c>
-      <c r="P2" t="n">
-        <v>20.0194214574241</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>16.6156155090355</v>
-      </c>
-      <c r="R2" t="n">
-        <v>14.6621958453669</v>
-      </c>
-      <c r="S2" t="n">
-        <v>2203136396.42027</v>
-      </c>
-      <c r="T2" t="n">
-        <v>7037463.92199608</v>
-      </c>
-      <c r="U2" t="n">
-        <v>11579100.4640944</v>
-      </c>
-      <c r="V2" t="n">
-        <v>-24251254.1480015</v>
-      </c>
-      <c r="W2" t="n">
-        <v>-11283151.7437972</v>
-      </c>
-      <c r="X2" t="n">
-        <v>2186218554.91457</v>
+      <c r="C2">
+        <v>376.47414082704699</v>
+      </c>
+      <c r="D2">
+        <v>366.64429991823903</v>
+      </c>
+      <c r="E2">
+        <v>310.94666006986</v>
+      </c>
+      <c r="F2">
+        <v>259.029500942303</v>
+      </c>
+      <c r="G2">
+        <v>224.26480320956301</v>
+      </c>
+      <c r="H2">
+        <v>209.33887650363999</v>
+      </c>
+      <c r="I2">
+        <v>201.87749926305301</v>
+      </c>
+      <c r="J2">
+        <v>197.80820832274699</v>
+      </c>
+      <c r="K2">
+        <v>27.650129146791699</v>
+      </c>
+      <c r="L2">
+        <v>27.530576734652101</v>
+      </c>
+      <c r="M2">
+        <v>24.1663053041623</v>
+      </c>
+      <c r="N2">
+        <v>20.021070559123899</v>
+      </c>
+      <c r="O2">
+        <v>17.225150107035901</v>
+      </c>
+      <c r="P2">
+        <v>15.979931241846399</v>
+      </c>
+      <c r="Q2">
+        <v>15.328849655582699</v>
+      </c>
+      <c r="R2">
+        <v>14.960858281551699</v>
+      </c>
+      <c r="S2" s="6">
+        <v>43798491.150945298</v>
+      </c>
+      <c r="T2" s="6">
+        <v>23594596.296174001</v>
+      </c>
+      <c r="U2" s="6">
+        <v>1098096.6501471801</v>
+      </c>
+      <c r="V2" s="6">
+        <v>-5330086.9346765596</v>
+      </c>
+      <c r="W2" s="6">
+        <v>-940603.57670762797</v>
+      </c>
+      <c r="X2" s="6">
+        <v>62220493.585882299</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>